<commit_message>
Parse multiple RichText values from shared strings
Some of the shared strings can contain multiple <r><t> elements
e.g.
<si> <r> <t> some </t> </r> <r> <t> value </r> </t> </si>

In order to correctly determine the entire contents of the string
it is necessary to parse all these values, and then combine them
into a single value.

The previous iteration of the sharedStrings parser did not handle
multiple r and t elements, so it has been updated to correctly
build the content in these cases.
</commit_message>
<xml_diff>
--- a/test/test-shared-strings-with-r-element.xlsx
+++ b/test/test-shared-strings-with-r-element.xlsx
@@ -35,7 +35,25 @@
         <color indexed="11"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
-      <t>sex</t>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="11"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>e</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="11"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>x</t>
     </r>
   </si>
 </sst>

</xml_diff>